<commit_message>
Add analysis code. Add thick border around most recently claimed area.
</commit_message>
<xml_diff>
--- a/Overzicht challenges Apeldoorn 04-05.xlsx
+++ b/Overzicht challenges Apeldoorn 04-05.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/thijs_vons_wur_nl/Documents/Thuis/RiskTagGame/RiskTagApeldoorn1904/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/thijs_vons_wur_nl/Documents/Thuis/RiskyRunApeldoorn0405/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="8_{5A8F5F9B-6B47-4BB9-90F5-12183F619251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30686A86-E20A-4393-A71A-1B98FA432F66}"/>
+  <xr:revisionPtr revIDLastSave="365" documentId="8_{5A8F5F9B-6B47-4BB9-90F5-12183F619251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F71BE7F-090C-4BC9-AA02-22457ED2E011}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1816A4B1-5691-498E-A51F-BAF9D2FFF305}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="155">
   <si>
     <t>Gebied Naam</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Verhaaltje Bij Challenge</t>
   </si>
   <si>
-    <t>Eet 500 kcal.</t>
-  </si>
-  <si>
     <t>Station</t>
   </si>
   <si>
@@ -200,18 +197,12 @@
     <t>Matendreef</t>
   </si>
   <si>
-    <t>52.218157, 5.949976</t>
-  </si>
-  <si>
     <t>52.209661, 5.953792</t>
   </si>
   <si>
     <t>52.204802, 5.952337</t>
   </si>
   <si>
-    <t>52.201851, 5.954012</t>
-  </si>
-  <si>
     <t>52.209283, 5.968970</t>
   </si>
   <si>
@@ -239,9 +230,6 @@
     <t>52.221880, 5.963997</t>
   </si>
   <si>
-    <t>52.222517, 5.959805</t>
-  </si>
-  <si>
     <t>Ietje Kooistraweg</t>
   </si>
   <si>
@@ -269,18 +257,12 @@
     <t>Vlijtsekade</t>
   </si>
   <si>
-    <t>Je bevindt je in het Wilhelminapark, een stadspark met invloeden van de Engelse landschapsstijl uit 1890. Zoek een bankje uit en geniet op dit bankje 5 minuten lang van dit park. (Stuur een foto aan het begin en einde van de 5 minuten)</t>
-  </si>
-  <si>
     <t>Geniet 5 minuten van het Wilhelminapark.</t>
   </si>
   <si>
     <t>Teken een Apeldoorns gebouw.</t>
   </si>
   <si>
-    <t>Je staat bij Het Potlood, een iconisch gebouw in Apeldoorn. Maar er zijn natuurlijk nog veel meer iconische gebouwen in Apeldoorn. Teken één van deze gebouwen. (Stuur een foto van de tekening. Ik moet het gebouw herkennen)</t>
-  </si>
-  <si>
     <t>Maak een foto van iemand die wij allebei kennen (die niks met het spel te maken heeft)</t>
   </si>
   <si>
@@ -290,111 +272,9 @@
     <t>52.218741, 5.971560</t>
   </si>
   <si>
-    <t>Treintijden weekend</t>
-  </si>
-  <si>
-    <t>Vertrektijd</t>
-  </si>
-  <si>
-    <t>xx:07</t>
-  </si>
-  <si>
-    <t>Eindstation</t>
-  </si>
-  <si>
-    <t>Eerste station</t>
-  </si>
-  <si>
-    <t>Zutphen</t>
-  </si>
-  <si>
-    <t>Apeldoorn de Maten</t>
-  </si>
-  <si>
-    <t>xx:23</t>
-  </si>
-  <si>
-    <t>Winterswijk</t>
-  </si>
-  <si>
-    <t>xx:14</t>
-  </si>
-  <si>
-    <t>Den Haag Centraal</t>
-  </si>
-  <si>
-    <t>Amersfoort Centraal</t>
-  </si>
-  <si>
-    <t>xx:30</t>
-  </si>
-  <si>
-    <t>Amsterdam Centraal</t>
-  </si>
-  <si>
-    <t>xx:44</t>
-  </si>
-  <si>
-    <t>xx:59</t>
-  </si>
-  <si>
-    <t>Internationale trein om het uur</t>
-  </si>
-  <si>
-    <t>xx:01</t>
-  </si>
-  <si>
-    <t>Om het uur</t>
-  </si>
-  <si>
-    <t>Staat een tijdje op het station?</t>
-  </si>
-  <si>
-    <t>xx:02</t>
-  </si>
-  <si>
-    <t>Deventer</t>
-  </si>
-  <si>
-    <t>Berlin Ostbahnhof/Deventer</t>
-  </si>
-  <si>
-    <t>xx:17</t>
-  </si>
-  <si>
-    <t>Enschede</t>
-  </si>
-  <si>
-    <t>xx:50</t>
-  </si>
-  <si>
-    <t>Almelo</t>
-  </si>
-  <si>
-    <t>Apeldoorn Osseveld</t>
-  </si>
-  <si>
-    <t>xx:47</t>
-  </si>
-  <si>
-    <t>xx:36</t>
-  </si>
-  <si>
-    <t>De Hofstede (Swen)</t>
-  </si>
-  <si>
-    <t>Badhuisweg (Mitchell)</t>
-  </si>
-  <si>
     <t>Arbeidstraat</t>
   </si>
   <si>
-    <t>Je staat nu aan de Arbeidstraat. Over arbeid gesproken, je zou wel kunnen zeggen dat dit spel op arbeid lijkt. Om goed jouw arbeid uit te kunnen voeren moet je natuurlijk wel voldoende eten. Eet daarom 500 kcal. (Stuur een foto van het product met de energie-informatie. En daarna foto's van het product vol en op)</t>
-  </si>
-  <si>
-    <t>Je staat op het Marktplein, wat een chaos zeg op zaterdag. Aangezien deze plek zo centraal is in Apeldoorn, moet jij nu een lijst maken met je 5 favoriete Apeldoorners, met een korte onderbouwing. (Stuur je lijst naar mij, ik moet je lijst goedkeuren voordat je door mag)</t>
-  </si>
-  <si>
     <t>Nieuw-Apostolische Kerk Apeldoorn</t>
   </si>
   <si>
@@ -404,12 +284,6 @@
     <t>Los de Wordle van vandaag op. (Maak een screenshot van het resultaat als bewijs. Open de pagina opnieuw, als het resultaat verdwijnt achter een menu)</t>
   </si>
   <si>
-    <t>Je staat bij het bijzonder teleurstellende station van Apeldoorn. Ga op een perron treinspotten: Maak een filmpje van een trein die aan komt rijden of weg rijdt, met enthousiast commentaar erbij. Extra gaaf als je ook nog ff de trein in gaat. Inspiratie: https://www.instagram.com/reel/CuCrt9_NV5V/?igsh=MXFqeDNoemlldzhlNQ==</t>
-  </si>
-  <si>
-    <t>Spring op de pogo stick van Mitchell.</t>
-  </si>
-  <si>
     <t>Restaurants Caterplein</t>
   </si>
   <si>
@@ -446,18 +320,9 @@
     <t>Maak muziek in de muziektent.</t>
   </si>
   <si>
-    <t>Maak een lijst van je favoriete Apeldoorners.</t>
-  </si>
-  <si>
-    <t>Eet voor €5.00 bij McDonalds.</t>
-  </si>
-  <si>
     <t>Doe een verdwenen beroep na.</t>
   </si>
   <si>
-    <t>Je bent aangekomen op de Vlijtsekade, gelegen aan het Apeldoorns kanaal. Verken het Apeldoorns kanaal door een rondje om het kanaal af te leggen (op een tempo dat je zelf kiest). Je moet over de Deventerstraat brug heen en over Het Sluisje. (Stuur een paar leuke foto's tussendoor als bewijs). Oh ja, je mag ook het kanaal in springen om de challenge te voltooien (er is een trappetje om het kanaal uit te klimmen)</t>
-  </si>
-  <si>
     <t>Tel het aantal restaurants op het Caterplein.</t>
   </si>
   <si>
@@ -473,57 +338,21 @@
     <t>Fotografeer een vogel.</t>
   </si>
   <si>
-    <t>Wat een schattig parkje zeg! Hier kun je heerlijk tot rust komen. Maar dat ga jij niet doen. Jij moet namelijk alle toestellen die in deze speeltuin staan maximaal gebruiken! (maak een filmpje van jezelf terwijl je alle toestellen in deze speeltuin maximaal gebruikt)</t>
-  </si>
-  <si>
-    <t>Vooruit, nog een laatste powerup voor de sfeer. Loop een supermarkt in en vind soepballetjes (rund, vega het mag allemaal), je hoeft het niet te kopen. De speler die dit als eerste doet mag meteen iemand naar keuze de tikker maken. (Deze tikker mag iedereen tikken, er is geen terugtik)</t>
-  </si>
-  <si>
     <t>Maak een selfie met iemand in uniform</t>
   </si>
   <si>
     <t>Gebruik de bus als vervoersmiddel</t>
   </si>
   <si>
-    <t>Wat zijn jullie veel aan het lopen zeg… Zou het niet fijn zijn als je de bus mag gebruiken. De persoon die als eerste een selfie maakt met iemand in uniform mag 2 keer de bus pakken (waarbij 1 keer telt als inchecken en uitchecken). De persoon die als tweede een selfie maakt met iemand in uniform mag 1 keer de bus pakken.</t>
-  </si>
-  <si>
     <t>Tenderlaan</t>
   </si>
   <si>
     <t>Maak een treingedicht.</t>
   </si>
   <si>
-    <t>Flip Kluin</t>
-  </si>
-  <si>
-    <t>Verken Flip Kluin.</t>
-  </si>
-  <si>
-    <t>Dierenspeciaalzaak Flip Kluin. Ik fietste hier altijd langs naar school, maar ben er nog nooit binnen geweest. Zou jij dat voor mij kunnen doen? Maak 5 foto's van dingen waarvan jij denkt dat ik ze graag zou willen hebben. (Stuur de foto's met korte beredenering als bewijs)</t>
-  </si>
-  <si>
-    <t>Asselsestraat (Imre)</t>
-  </si>
-  <si>
-    <t>Louisalaan</t>
-  </si>
-  <si>
-    <t>Voorzie de host van een snack.</t>
-  </si>
-  <si>
-    <t>Je staat voor het huis van Douwe, waar ik toevallig ook ben! Ik ben heel hard aan het werk op dit spel in goede banen te leiden. Daarom verdien ik wel een snackje. Voorzie mij van een lekker snackje. (Als je heel lief vraagt mag je misschien mijn fiets lenen)</t>
-  </si>
-  <si>
-    <t>52.207436, 5.931227</t>
-  </si>
-  <si>
     <t>52.213136, 5.952308</t>
   </si>
   <si>
-    <t>52.202680, 5.964226</t>
-  </si>
-  <si>
     <t>52.207350, 5.962194</t>
   </si>
   <si>
@@ -545,58 +374,133 @@
     <t>Je bent aangekomen in De Maten, om precies te zijn, Matendreef. De straten om je heen zijn allemaal vernoemd naar verdwenen beroepen (Looiersdreef, Postmeestersdreef, etc.). Beeld één van deze beroepen uit, door minstens 2 attributen te gebruiken. (Stuur een foto of filmpje als bewijs)</t>
   </si>
   <si>
-    <t>Je staat hier bij de spoorwegovergang waar Swen ons altijd verliet als we naar huis fietsten vanuit school :(. Maar wist je dat hier in de buurt ooit het Koningslijntje liep? Vind het monument dat is neergelegd om het Koningslijntje te herdenken. (Stuur er een foto van als bewijs)</t>
-  </si>
-  <si>
-    <t>En het 3e uur is al weer voltooid. Tijd voor een powerup! Degene die de als eerste een frikandelbroodje op eet mag het volgende gebied dat diegene claimt vastzetten. Dit betekent dat niemand anders dit gebied meer kan claimen. (Stuur een foto van de eerste en laatste hap als bewijs)</t>
-  </si>
-  <si>
-    <t>Pfoeh, dat was een flink eind lopen. Nu maar hopen dat je deze challenge kunt halen… Vind dat guitige koppie van Imre en win een potje Uno van hem.</t>
-  </si>
-  <si>
-    <t>Je bevindt je in de vogelbuurt, waar veel van de namen van straten vernoemd naar een vogel zijn. Volgens mij kunt jij wel een diepere connectie met de vogelbuurt gebruiken. Maak daarom een foto van een echte, levende vogel. (Stuur de foto als bewijs)</t>
-  </si>
-  <si>
-    <t>Wat een mooi pleintje hier aan de Tenderlaan zeg. Wist jij dat een tender een wagen achter een stoomlocomotief is waarin brandstof en water vervoerd worden? Het is geen toeval dat deze straat zo heet, want alle straatnamen zijn in het treinthema. Schrijf een gedicht van minimaal 6 regels waar je het onderwerp van minstens 2 straatnamen om je heen verwerkt. (Stuur het gedicht op)</t>
-  </si>
-  <si>
-    <t>De Hoofdstraat, de langste winkelstraat van Nederland (Of nee, toch niet. Blijkbaar is er een winkelstraat in Dordrecht 70 meter langer… ). Anyway, je zult vast honger hebben. Koop voor €5.00 aan producten bij de McDonalds en eet dit op. (Stuur een foto van het bonnetje, en foto's van het product vol en op)</t>
-  </si>
-  <si>
-    <t>Wat een mooie kerk is de Nieuw-Apostolische Kerk Apeldoorn zeg! Meer mensen moeten kennis hebben over deze kerk. Daarom moet jij een voorbijganger een feitje vertellen over de kerk. Het feitje moet feitelijk correct zijn en over de kerk gaan. (Doe een poging om een video of audio-opname te maken als bewijs)</t>
-  </si>
-  <si>
-    <t>Deze muziektent is een replica van de originele muziektent die in 1960 is afgebrand. Om de traditie van muziek in het Oranjepark hoog te houden moet jij muziek maken in (of bij) de muziektent. Dit muzikale meesterwerk moet minstens 1 minuut lang zijn, wees creatief! (Stuur een filmpje van jouw muzikale creatie als bewijs)</t>
-  </si>
-  <si>
-    <t>Dit is het brugklasgebouw van Mheenpark (als het goed is). Bij de middelbare school horen natuurlijk klassenfoto's. En dat is precies wat jij gaat maken; een klassenfoto met minstens 10 leerlingen. Maak met spullen die je in het park vind 'leerlingen'. Of vind echte mensen, dat mag ook. (Stuur een foto van je klassenfoto als bewijs)</t>
-  </si>
-  <si>
     <t>Spoorwegovergang</t>
   </si>
   <si>
-    <t>Speel spelletjes met Swen.</t>
-  </si>
-  <si>
-    <t>Je bent aangekomen bij Swen. Helaas mag je niet naar binnen, want Carola is een grote schoonmaak aan het doen. Daarom ga je buiten spelletjes spelen met Swen. Win een potje Jeu de Boule van Swen en speel daarna één van de twee overgooi spelletjes. Je moet 20 keer achter elkaar succesvol overgooien met Swen. (Swen is het onafhankelijke bewijs dat je de challenge voltooid hebt)</t>
-  </si>
-  <si>
     <t>https://travle.earth/benelux, https://globle-game.com/game</t>
   </si>
   <si>
-    <t>Alweer twee uur bezig, hebben jullie er nog zin in? Maak je op voor de tweede powerup. De powerup is dat je een persoon naar keuze voor 10 minuten stil mag laten staan. Dit mag je op elk moment voor de rest van het spel doen. Degene die als eerste een foto van een gele auto maakt wint deze powerup.</t>
-  </si>
-  <si>
-    <t>Badhuisweg 36, de uitvalsbasis van Mitchell Berends. Omdat Mitchell zo'n gentleman is heeft hij voor dit spel zijn pogostick beschikbaar gesteld (achter de plantenbak). Leg in één keer een afstand af van 2 auto's op de pogostick. (Maak hier een filmpje van als bewijs. Het is waarschijnlijk het makkelijkst om je telefoon al filmend ergens neer te zetten).</t>
-  </si>
-  <si>
     <t>52.205553, 5.971737</t>
   </si>
   <si>
     <t>Het Caterplein, officieel niet eens een plein, maar het is er altijd gezellig. Maak een lijst met de restaurants die je kunt zien vanaf de boom midden op het plein (clubs tellen dus niet mee).</t>
   </si>
   <si>
-    <t>Win een potje pesten van Imre</t>
+    <t>52.220283, 5.948324</t>
+  </si>
+  <si>
+    <t>Soerenseweg 19 (Mark)</t>
+  </si>
+  <si>
+    <t>52.224323, 5.961342</t>
+  </si>
+  <si>
+    <t>52.200153, 5.954616</t>
+  </si>
+  <si>
+    <t>De Ploeg</t>
+  </si>
+  <si>
+    <t>52.209215, 5.935223</t>
+  </si>
+  <si>
+    <t>Jachthoornlaan</t>
+  </si>
+  <si>
+    <t>Eet 1000 kcal.</t>
+  </si>
+  <si>
+    <t>Jullie staan nu aan de Arbeidstraat. Over arbeid gesproken, je zou wel kunnen zeggen dat dit spel op arbeid lijkt. Om goed jullie arbeid uit te kunnen voeren moeten jullie natuurlijk wel voldoende eten. Eet daarom in totaal 1000 kcal. (Stuur een foto van de producten met de energie-informatie. En daarna foto's van de producten vol en op)</t>
+  </si>
+  <si>
+    <t>Doe shotjes bij een school.</t>
+  </si>
+  <si>
+    <t>De locatie van Veluws College Walterbosch aan de Jachthoornlaan. Dat is natuurlijk een school, de perfect plek voor shotjes! Neem 3 shotjes van drank tussen 10% en 25% of 2 shotjes van 25%+ drank.</t>
+  </si>
+  <si>
+    <t>Wat een schattig parkje zeg! Hier kun je heerlijk tot rust komen. Maar dat gaan jullie niet doen. Eén van jullie moet namelijk alle toestellen die in deze speeltuin staan maximaal gebruiken! (de ander maakt hier een mooie videorapportage van)</t>
+  </si>
+  <si>
+    <t>Je staat hier bij de spoorwegovergang waar Swen ons altijd verliet als we naar huis fietsten vanuit school :(. Maar wisten jullie dat hier in de buurt ooit het Koningslijntje liep? Vind het monument dat is neergelegd om het Koningslijntje te herdenken. (Stuur er een foto van als bewijs)</t>
+  </si>
+  <si>
+    <t>Jullie bevinden je in de vogelbuurt, waar veel van de namen van straten vernoemd naar een vogel zijn. Volgens mij kunnen jullie wel een diepere connectie met de vogelbuurt gebruiken. Maak daarom een foto van een echte, levende vogel. (Stuur de foto als bewijs)</t>
+  </si>
+  <si>
+    <t>Wat een mooi pleintje hier aan de Tenderlaan zeg. Wisten jullie dat een tender een wagen achter een stoomlocomotief is waarin brandstof en water vervoerd worden? Het is geen toeval dat deze straat zo heet, want alle straatnamen hier zijn in het treinthema. Schrijf een gedicht van minimaal 6 regels waar jullie het onderwerp van minstens 2 straatnamen om je heen verwerken. (Stuur het gedicht op)</t>
+  </si>
+  <si>
+    <t>Jullie staan bij het bijzonder teleurstellende station van Apeldoorn. Ga op een perron treinspotten: Maak een filmpje van een trein die aan komt rijden of weg rijdt, met enthousiast commentaar erbij. Extra gaaf als jullie ook nog ff de trein in gaan. Inspiratie: https://www.instagram.com/reel/CuCrt9_NV5V/?igsh=MXFqeDNoemlldzhlNQ==</t>
+  </si>
+  <si>
+    <t>Jullie staan bij Het Potlood, een iconisch gebouw in Apeldoorn. Maar er zijn natuurlijk nog veel meer iconische gebouwen in Apeldoorn. Teken één van deze gebouwen op papier. (Stuur een foto van de tekening. Ik moet het gebouw herkennen)</t>
+  </si>
+  <si>
+    <t>De Hoofdstraat, de langste winkelstraat van Nederland (Of nee, toch niet. Blijkbaar is er een winkelstraat in Dordrecht 70 meter langer… ). Anyway, je zult vast honger hebben. Koop voor €10.00 aan producten bij de McDonalds en eet dit op. (Stuur een foto van het bonnetje, en foto's van de producten vol en op)</t>
+  </si>
+  <si>
+    <t>Jullie staan op het Marktplein, met als grote trots de Markthal. Aangezien deze plek zo centraal is in Apeldoorn, moeten jullie nu een lijst maken met jullie 5 favoriete Apeldoorners, met een korte onderbouwing. (Stuur jullie lijst naar mij, ik moet jullie lijst goedkeuren voordat jullie door mogen)</t>
+  </si>
+  <si>
+    <t>Wat een mooie kerk is de Nieuw-Apostolische Kerk Apeldoorn zeg! Meer mensen moeten kennis hebben over deze kerk. Daarom moeten jullie een voorbijganger een feitje vertellen over de kerk. Het feitje moet feitelijk correct zijn en over de kerk gaan. (Maak een video of audio-opname als bewijs)</t>
+  </si>
+  <si>
+    <t>Deze muziektent is een replica van de originele muziektent die in 1960 is afgebrand. Om de traditie van muziek in het Oranjepark hoog te houden moeten jullie muziek maken in (of bij) de muziektent. Dit muzikale meesterwerk moet minstens 1 minuut lang zijn, wees creatief! (Stuur een filmpje van jouw muzikale creatie als bewijs)</t>
+  </si>
+  <si>
+    <t>Eet voor €10.00 bij McDonalds.</t>
+  </si>
+  <si>
+    <t>Haal een snack voor de host bij de Spar.</t>
+  </si>
+  <si>
+    <t>Wat toevallig zeg, jullie staan bij het huis waar ik nu ben, kom maar even binnen!</t>
+  </si>
+  <si>
+    <t>Emma Plein</t>
+  </si>
+  <si>
+    <t>Speel koning(in) en lakei</t>
+  </si>
+  <si>
+    <t>Jullie bevinden je in een koninlijke buurt (als het aan de straatnamen ligt tenminste). Maak 5 scènes van minstens 20 seconde waarin één iemand de koning(in) is en de ander een lakei. De koning(in) geeft de lakei een opdracht die uitgevoerd moet worden. (Stuur filmpjes als bewijs)</t>
+  </si>
+  <si>
+    <t>Jullie bevinden je in het Wilhelminapark, een stadspark met invloeden van de Engelse landschapsstijl uit 1890. Zoek een bankje uit en geniet op dit bankje 5 minuten lang van dit park. (Stuur een foto aan het begin en einde van de 5 minuten)</t>
+  </si>
+  <si>
+    <t>Jullie zijn aangekomen op de Vlijtsekade, gelegen aan het Apeldoorns kanaal. Verken het Apeldoorns kanaal door een rondje om het kanaal af te leggen (op een tempo dat jullie zelf kiezen). Jullie moeten over de Deventerstraat brug heen en over Het Sluisje. (Stuur een paar leuke foto's tussendoor als bewijs). Oh ja, één van jullie mag ook het kanaal in springen om de challenge te voltooien (er is een trappetje om het kanaal uit te klimmen)</t>
+  </si>
+  <si>
+    <t>Dit is het brugklasgebouw van Mheenpark. Bij de middelbare school horen natuurlijk klassenfoto's. En dat is precies wat jullie gaan maken; een klassenfoto met minstens 10 leerlingen. Maak met spullen die jullie in het park vinden 'leerlingen'. Of vind echte mensen, dat mag ook. (Stuur een foto van jullie klassenfoto als bewijs)</t>
+  </si>
+  <si>
+    <t>Wat zijn jullie veel aan het lopen zeg… Zou het niet fijn zijn als jullie de bus mogen gebruiken. Het team dat als eerste een selfie maakt met iemand in uniform mag 2 keer de bus pakken (waarbij 1 keer telt als inchecken en uitchecken). Het team dat als tweede een selfie maakt met iemand in uniform mag 1 keer de bus pakken.</t>
+  </si>
+  <si>
+    <t>Alweer twee uur bezig, hebben jullie er nog zin in? Maak je op voor de tweede powerup. De powerup is dat je een team naar keuze voor 10 minuten stil mag laten staan. Dit mogen jullie op elk moment voor de rest van het spel doen. Het team dat als eerste een foto van een gele auto maakt wint deze powerup.</t>
+  </si>
+  <si>
+    <t>En het 3e uur is al weer voltooid. Tijd voor een powerup! Het team dat als eerste 2 frikandelbroodjes op eet mag het volgende gebied dat het team claimt vastzetten. Dit betekent dat niemand anders dit gebied meer kan claimen. (Stuur een foto van de eerste en laatste hap als bewijs)</t>
+  </si>
+  <si>
+    <t>Vooruit, nog een laatste powerup voor de sfeer. Loop een supermarkt in en vind soepballetjes (rund, vega het mag allemaal), jullie hoeven het niet te kopen. Het team die dit als eerste doet mag meteen een ander team naar keuze de tikker maken. (De nieuwe tikker heeft geen terugtik, het team mag iedereen tikken)</t>
+  </si>
+  <si>
+    <t>Maak een lijst van jullie favoriete Apeldoorners.</t>
+  </si>
+  <si>
+    <t>52.203600, 5.964513</t>
+  </si>
+  <si>
+    <t>Meerkoetweg x Adelaarslaan</t>
+  </si>
+  <si>
+    <t>Herdenk de vrijheid.</t>
+  </si>
+  <si>
+    <t>Het is vandaag 4 mei en morgen 5 mei. Omdat dit twee belangrijke dagen zijn om de Nederlandse geschiedenis te herdenken gaan jullie dit alvast doen. Wees eerst twee minuten stil en houd daarna een speech van minimaal 1 minuut over de vrijheid in Nederland. (Stuur een filmpje als bewijs)</t>
   </si>
 </sst>
 </file>
@@ -993,7 +897,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,133 +934,127 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>125</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>183</v>
+        <v>117</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G7" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
         <v>152</v>
@@ -1170,622 +1068,481 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>137</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="F16">
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
+      </c>
+      <c r="E19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="F20" t="s">
-        <v>181</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
         <v>76</v>
       </c>
-      <c r="E21" t="s">
-        <v>82</v>
-      </c>
       <c r="G21" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="G22" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
         <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
         <v>14</v>
       </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
       <c r="G28" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
         <v>17</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>21</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>22</v>
       </c>
-      <c r="E30" t="s">
-        <v>23</v>
-      </c>
       <c r="G30" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
         <v>28</v>
-      </c>
-      <c r="C38" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
         <v>31</v>
       </c>
-      <c r="C40" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="E47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
         <v>84</v>
       </c>
-      <c r="E47" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
         <v>85</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="E51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
         <v>87</v>
       </c>
-      <c r="C48" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
         <v>88</v>
       </c>
-      <c r="E48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" t="s">
-        <v>95</v>
-      </c>
-      <c r="D49" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>104</v>
-      </c>
-      <c r="B50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" t="s">
-        <v>105</v>
-      </c>
-      <c r="E50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
         <v>89</v>
       </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
         <v>90</v>
-      </c>
-      <c r="D51" t="s">
-        <v>103</v>
-      </c>
-      <c r="E51" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>93</v>
-      </c>
-      <c r="B52" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" t="s">
-        <v>95</v>
-      </c>
-      <c r="E52" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>98</v>
-      </c>
-      <c r="B57" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" t="s">
-        <v>108</v>
-      </c>
-      <c r="C58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>109</v>
-      </c>
-      <c r="B59" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" t="s">
-        <v>111</v>
-      </c>
-      <c r="E59" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes to analysis python file
</commit_message>
<xml_diff>
--- a/Overzicht challenges Apeldoorn 04-05.xlsx
+++ b/Overzicht challenges Apeldoorn 04-05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/thijs_vons_wur_nl/Documents/Thuis/RiskyRunApeldoorn0405/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="8_{5A8F5F9B-6B47-4BB9-90F5-12183F619251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD5E009B-5BD6-4F27-9BC7-00836173228A}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{5A8F5F9B-6B47-4BB9-90F5-12183F619251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5657869-E0BD-4CB8-8CA9-B563D60E7780}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1816A4B1-5691-498E-A51F-BAF9D2FFF305}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1816A4B1-5691-498E-A51F-BAF9D2FFF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
   <si>
     <t>Gebied Naam</t>
   </si>
@@ -77,9 +77,6 @@
     <t>1 uur</t>
   </si>
   <si>
-    <t>Laat iemand 10 minuten stil staan (niet de tikker)</t>
-  </si>
-  <si>
     <t>Spot een gele auto</t>
   </si>
   <si>
@@ -92,15 +89,9 @@
     <t>Het volgende gebied dat je claimt kan niet meer afgepakt worden</t>
   </si>
   <si>
-    <t>Eet een frikandelbroodje</t>
-  </si>
-  <si>
     <t>3.5 uur</t>
   </si>
   <si>
-    <t>Je mag een gebied naar keuze van jezelf vastzetten</t>
-  </si>
-  <si>
     <t>Je mag de tikker wisselen naar keuze</t>
   </si>
   <si>
@@ -263,9 +254,6 @@
     <t>Teken een Apeldoorns gebouw.</t>
   </si>
   <si>
-    <t>Maak een foto van iemand die wij allebei kennen (die niks met het spel te maken heeft)</t>
-  </si>
-  <si>
     <t>Ren een rondje om het kanaal.</t>
   </si>
   <si>
@@ -284,48 +272,12 @@
     <t>Los de Wordle van vandaag op. (Maak een screenshot van het resultaat als bewijs. Open de pagina opnieuw, als het resultaat verdwijnt achter een menu)</t>
   </si>
   <si>
-    <t>Restaurants Caterplein</t>
-  </si>
-  <si>
-    <t>De Graaf van Vlaanderen</t>
-  </si>
-  <si>
-    <t>YuMe</t>
-  </si>
-  <si>
-    <t>Finnegans</t>
-  </si>
-  <si>
-    <t>Nobel &amp; Wijn</t>
-  </si>
-  <si>
-    <t>De Babbel</t>
-  </si>
-  <si>
-    <t>De Trap</t>
-  </si>
-  <si>
-    <t>Le Baffon (wel ver weg)</t>
-  </si>
-  <si>
-    <t>Crazy Italian (wel ver weg)</t>
-  </si>
-  <si>
-    <t>Mazar (niet zichbaar)</t>
-  </si>
-  <si>
-    <t>Pibia (niet zichtbaar0</t>
-  </si>
-  <si>
     <t>Maak muziek in de muziektent.</t>
   </si>
   <si>
     <t>Doe een verdwenen beroep na.</t>
   </si>
   <si>
-    <t>Tel het aantal restaurants op het Caterplein.</t>
-  </si>
-  <si>
     <t>Vertel iemand een feitje over de kerk.</t>
   </si>
   <si>
@@ -335,9 +287,6 @@
     <t>Vogelbuurt</t>
   </si>
   <si>
-    <t>Fotografeer een vogel.</t>
-  </si>
-  <si>
     <t>Maak een selfie met iemand in uniform</t>
   </si>
   <si>
@@ -383,9 +332,6 @@
     <t>52.205553, 5.971737</t>
   </si>
   <si>
-    <t>Het Caterplein, officieel niet eens een plein, maar het is er altijd gezellig. Maak een lijst met de restaurants die je kunt zien vanaf de boom midden op het plein (clubs tellen dus niet mee).</t>
-  </si>
-  <si>
     <t>52.220283, 5.948324</t>
   </si>
   <si>
@@ -419,12 +365,6 @@
     <t>Wat een schattig parkje zeg! Hier kun je heerlijk tot rust komen. Maar dat gaan jullie niet doen. Eén van jullie moet namelijk alle toestellen die in deze speeltuin staan maximaal gebruiken! (de ander maakt hier een mooie videorapportage van)</t>
   </si>
   <si>
-    <t>Je staat hier bij de spoorwegovergang waar Swen ons altijd verliet als we naar huis fietsten vanuit school :(. Maar wisten jullie dat hier in de buurt ooit het Koningslijntje liep? Vind het monument dat is neergelegd om het Koningslijntje te herdenken. (Stuur er een foto van als bewijs)</t>
-  </si>
-  <si>
-    <t>Jullie bevinden je in de vogelbuurt, waar veel van de namen van straten vernoemd naar een vogel zijn. Volgens mij kunnen jullie wel een diepere connectie met de vogelbuurt gebruiken. Maak daarom een foto van een echte, levende vogel. (Stuur de foto als bewijs)</t>
-  </si>
-  <si>
     <t>Wat een mooi pleintje hier aan de Tenderlaan zeg. Wisten jullie dat een tender een wagen achter een stoomlocomotief is waarin brandstof en water vervoerd worden? Het is geen toeval dat deze straat zo heet, want alle straatnamen hier zijn in het treinthema. Schrijf een gedicht van minimaal 6 regels waar jullie het onderwerp van minstens 2 straatnamen om je heen verwerken. (Stuur het gedicht op)</t>
   </si>
   <si>
@@ -443,27 +383,18 @@
     <t>Wat een mooie kerk is de Nieuw-Apostolische Kerk Apeldoorn zeg! Meer mensen moeten kennis hebben over deze kerk. Daarom moeten jullie een voorbijganger een feitje vertellen over de kerk. Het feitje moet feitelijk correct zijn en over de kerk gaan. (Maak een video of audio-opname als bewijs)</t>
   </si>
   <si>
-    <t>Deze muziektent is een replica van de originele muziektent die in 1960 is afgebrand. Om de traditie van muziek in het Oranjepark hoog te houden moeten jullie muziek maken in (of bij) de muziektent. Dit muzikale meesterwerk moet minstens 1 minuut lang zijn, wees creatief! (Stuur een filmpje van jouw muzikale creatie als bewijs)</t>
-  </si>
-  <si>
     <t>Eet voor €10.00 bij McDonalds.</t>
   </si>
   <si>
     <t>Haal een snack voor de host bij de Spar.</t>
   </si>
   <si>
-    <t>Wat toevallig zeg, jullie staan bij het huis waar ik nu ben, kom maar even binnen!</t>
-  </si>
-  <si>
     <t>Emma Plein</t>
   </si>
   <si>
     <t>Speel koning(in) en lakei</t>
   </si>
   <si>
-    <t>Jullie bevinden je in een koninlijke buurt (als het aan de straatnamen ligt tenminste). Maak 5 scènes van minstens 20 seconde waarin één iemand de koning(in) is en de ander een lakei. De koning(in) geeft de lakei een opdracht die uitgevoerd moet worden. (Stuur filmpjes als bewijs)</t>
-  </si>
-  <si>
     <t>Jullie bevinden je in het Wilhelminapark, een stadspark met invloeden van de Engelse landschapsstijl uit 1890. Zoek een bankje uit en geniet op dit bankje 5 minuten lang van dit park. (Stuur een foto aan het begin en einde van de 5 minuten)</t>
   </si>
   <si>
@@ -479,12 +410,6 @@
     <t>Alweer twee uur bezig, hebben jullie er nog zin in? Maak je op voor de tweede powerup. De powerup is dat je een team naar keuze voor 10 minuten stil mag laten staan. Dit mogen jullie op elk moment voor de rest van het spel doen. Het team dat als eerste een foto van een gele auto maakt wint deze powerup.</t>
   </si>
   <si>
-    <t>En het 3e uur is al weer voltooid. Tijd voor een powerup! Het team dat als eerste 2 frikandelbroodjes op eet mag het volgende gebied dat het team claimt vastzetten. Dit betekent dat niemand anders dit gebied meer kan claimen. (Stuur een foto van de eerste en laatste hap als bewijs)</t>
-  </si>
-  <si>
-    <t>Vooruit, nog een laatste powerup voor de sfeer. Loop een supermarkt in en vind soepballetjes (rund, vega het mag allemaal), jullie hoeven het niet te kopen. Het team die dit als eerste doet mag meteen een ander team naar keuze de tikker maken. (De nieuwe tikker heeft geen terugtik, het team mag iedereen tikken)</t>
-  </si>
-  <si>
     <t>Maak een lijst van jullie favoriete Apeldoorners.</t>
   </si>
   <si>
@@ -497,10 +422,55 @@
     <t>Herdenk de vrijheid.</t>
   </si>
   <si>
-    <t>Het is vandaag 4 mei en morgen 5 mei. Omdat dit twee belangrijke dagen zijn om de Nederlandse geschiedenis te herdenken gaan jullie dit alvast doen. Wees eerst twee minuten stil en houd daarna een speech van minimaal 1 minuut over de vrijheid in Nederland. (Stuur een filmpje als bewijs)</t>
-  </si>
-  <si>
-    <t>De locatie van Veluws College Walterbosch aan de Jachthoornlaan. Dat is natuurlijk een school, de perfect plek voor shotjes! Neem 3 shotjes van drank tussen 10% en 25% of 2 shotjes van 25%+ drank. Een shotje is 30 mL. (Stuur een filmpje als bewijs)</t>
+    <t>Het Caterplein, officieel niet eens een plein, maar het is er altijd gezellig. Aangezien het vandaag heerlijk weer is (oh nee, toch niet), moeten jullie één drankje bestellen op het terras en dat drankje opdrinken. (Stuur een foto van het drankje vol en leeg)</t>
+  </si>
+  <si>
+    <t>Drink een drankje aan het Caterplein.</t>
+  </si>
+  <si>
+    <t>Laat iemand 10 minuten stil staan</t>
+  </si>
+  <si>
+    <t>De locatie van Veluws College Walterbosch aan de Jachthoornlaan. Dat is natuurlijk een school, de perfect plek voor shotjes! Neem 4 shotjes van drank tussen 10% en 20%, 3 shotjes van drank tusen 20 en 30% of 2 shotjes van 30%+ drank. Een shotje is minimaal 30 mL. (Stuur een filmpje als bewijs)</t>
+  </si>
+  <si>
+    <t>En het 3e uur is al weer voltooid. Tijd voor een powerup! De powerup is dat het volgende gebied dat het team overneemt vergrendeld wordt, niemand anders kan dat gebied dan meer overnemen. Het team dat als eerste twee shotjes doet wint deze powerup. Een shotje is minimaal 30 mL. (Stuur een filmpje als bewijs)</t>
+  </si>
+  <si>
+    <t>Speel steen, papier, schaar tegen AI.</t>
+  </si>
+  <si>
+    <t>Doe 2 shotjes</t>
+  </si>
+  <si>
+    <t>Wat toevallig zeg, jullie staan bij het huis waar de host nu is. Aangezien de host zo hard aan het werk is moeten jullie hem voorzien van een snackje. Haal een snack bij de Spar en breng dit naar de host.</t>
+  </si>
+  <si>
+    <t>Jullie staan hier bij de spoorwegovergang waar Swen ons altijd verliet als we naar huis fietsten vanuit school :(. Maar wisten jullie dat hier in de buurt ooit het Koningslijntje liep? Vind het monument dat is neergelegd om het Koningslijntje te herdenken. (Stuur er een foto van als bewijs)</t>
+  </si>
+  <si>
+    <t>Jullie bevinden je in de vogelbuurt, waar veel van de namen van straten vernoemd naar een vogel zijn. Volgens mij kunnen jullie wel een diepere connectie met de vogelbuurt gebruiken. Maak daarom een 10 seconde filmpje van een levende vogel. (Stuur het filmpje als bewijs)</t>
+  </si>
+  <si>
+    <t>Film een vogel.</t>
+  </si>
+  <si>
+    <t>Het is vandaag 4 mei en morgen 5 mei. Omdat dit twee belangrijke dagen zijn om de Nederlandse geschiedenis te herdenken en de vrijheid te vieren gaan jullie dit alvast doen. Wees eerst twee minuten stil en houd daarna een speech van minimaal 30 seconde over de vrijheid in Nederland. (Stuur een filmpje als bewijs, je hoeft niet persé een filmpje van twee minuten stil te sturen)</t>
+  </si>
+  <si>
+    <t>Deze plek is perfect voor een leuk spelletje. En wat is nou leuker dan een spelletje spelen tegen ChatGPT. Win een potje steen, papier, schaar van ChatGPT. Eén potje is best of 11 (dus 6 winnen) en jullie moeten als eerste spelen. (Stuur screenshots als bewijs)</t>
+  </si>
+  <si>
+    <t>Maak een foto van iemand die wij allebei kennen (die niks met het spel te maken heeft). Je mag niet aanbellen bij een huis hiervoor</t>
+  </si>
+  <si>
+    <t>Jullie bevinden je in een koninklijke buurt (als het aan de straatnamen ligt tenminste). Maak 3 sketches van minstens 20 seconde waarin één iemand de koning(in) is en de ander een lakei. De koning(in) geeft de lakei een opdracht die uitgevoerd moet worden. (Stuur filmpjes als bewijs)</t>
+  </si>
+  <si>
+    <t>Deze muziektent is een replica van de originele muziektent die in 1960 is afgebrand. Om de traditie van muziek in het Oranjepark hoog te houden moeten jullie muziek maken in (of bij) de muziektent. Dit muzikale meesterwerk moet minstens 1 minuut lang zijn, wees creatief! (Stuur een filmpje van jullie muzikale creatie als bewijs)</t>
+  </si>
+  <si>
+    <t>Vooruit, nog een laatste powerup voor de sfeer. Loop een supermarkt in en vind soepballetjes (rund, vega het mag allemaal), jullie hoeven het niet te kopen. Het team dat dit als eerste doet mag meteen een ander team naar keuze de tikker maken. (De nieuwe tikker heeft geen terugtik; dat team mag iedereen tikken)</t>
   </si>
 </sst>
 </file>
@@ -894,22 +864,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5180A3-82A3-4F3F-BA53-BD0E6DEE68AE}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,181 +902,187 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="G8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1114,265 +1090,262 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
       <c r="G18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" t="s">
-        <v>139</v>
-      </c>
-      <c r="E19" t="s">
-        <v>140</v>
-      </c>
       <c r="G19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F20" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
         <v>72</v>
       </c>
-      <c r="E21" t="s">
-        <v>76</v>
-      </c>
       <c r="G21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
         <v>94</v>
       </c>
-      <c r="G23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1386,164 +1359,108 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="B30" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="E30" t="s">
         <v>19</v>
       </c>
-      <c r="B30" t="s">
+      <c r="G30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E30" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="C38" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>27</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E49" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
-      <c r="E51" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E59" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E62" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E63" t="s">
-        <v>92</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>